<commit_message>
Revert "Revert "Update template-cms-sidak""
This reverts commit 5de9552fde7af16424481d81b202ee24d1fd8a18.
</commit_message>
<xml_diff>
--- a/public/template-cms-sidak.xlsx
+++ b/public/template-cms-sidak.xlsx
@@ -1,28 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\test-laravel\digitalisasi-rt-rw-laravel\public\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory List" sheetId="1" r:id="rId1"/>
+    <sheet name="Gender-List" sheetId="2" r:id="rId2"/>
+    <sheet name="Religion-List" sheetId="3" r:id="rId3"/>
+    <sheet name="Job-List" sheetId="4" r:id="rId4"/>
+    <sheet name="Pendidikan-List" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="valHighlight">'Inventory List'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
   <si>
     <t>No KTP</t>
   </si>
@@ -91,13 +90,109 @@
   </si>
   <si>
     <t>2020-08-23 00:00:00</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Keterangan</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>ISLAM</t>
+  </si>
+  <si>
+    <t>Budha</t>
+  </si>
+  <si>
+    <t>Katolik</t>
+  </si>
+  <si>
+    <t>Hindu</t>
+  </si>
+  <si>
+    <t>Kristen</t>
+  </si>
+  <si>
+    <t>Kong Hu Chu</t>
+  </si>
+  <si>
+    <t>Lain - Lain</t>
+  </si>
+  <si>
+    <t>Pelajar/Mahasiswa</t>
+  </si>
+  <si>
+    <t>Wirausaha</t>
+  </si>
+  <si>
+    <t>TNI</t>
+  </si>
+  <si>
+    <t>KARYAWAN SWASTA</t>
+  </si>
+  <si>
+    <t>Ibu Rumah Tangga</t>
+  </si>
+  <si>
+    <t>Guru</t>
+  </si>
+  <si>
+    <t>Belum Bekerja</t>
+  </si>
+  <si>
+    <t>Pegawai Negri Sipil</t>
+  </si>
+  <si>
+    <t>Pengacara</t>
+  </si>
+  <si>
+    <t>Karyawan BUMN</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>SMPN</t>
+  </si>
+  <si>
+    <t>SMA/SMK</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>SMP</t>
+  </si>
+  <si>
+    <t>TK</t>
+  </si>
+  <si>
+    <t>PAUD</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -111,15 +206,21 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -127,11 +228,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -142,27 +258,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="23">
-    <dxf>
-      <font>
-        <strike/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -268,6 +370,22 @@
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -353,28 +471,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblInventoryList" displayName="tblInventoryList" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblInventoryList" displayName="tblInventoryList" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="17">
   <autoFilter ref="A1:Q2"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="No KTP" dataDxfId="18"/>
-    <tableColumn id="2" name="No KK" dataDxfId="17"/>
-    <tableColumn id="3" name="First Name" dataDxfId="16"/>
-    <tableColumn id="4" name="Last Name" dataDxfId="15"/>
-    <tableColumn id="5" name="Gender" dataDxfId="14"/>
-    <tableColumn id="11" name="Religion" dataDxfId="13">
+    <tableColumn id="1" name="No KTP" dataDxfId="16"/>
+    <tableColumn id="2" name="No KK" dataDxfId="15"/>
+    <tableColumn id="3" name="First Name" dataDxfId="14"/>
+    <tableColumn id="4" name="Last Name" dataDxfId="13"/>
+    <tableColumn id="5" name="Gender" dataDxfId="12"/>
+    <tableColumn id="11" name="Religion" dataDxfId="11">
       <calculatedColumnFormula>tblInventoryList[[#This Row],[Last Name]]*tblInventoryList[[#This Row],[Gender]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Address" dataDxfId="12"/>
-    <tableColumn id="7" name="Address Code" dataDxfId="11"/>
-    <tableColumn id="8" name="Job" dataDxfId="10"/>
-    <tableColumn id="9" name="Salary Range" dataDxfId="9"/>
-    <tableColumn id="10" name="Phone" dataDxfId="8"/>
-    <tableColumn id="12" name="Email" dataDxfId="7"/>
-    <tableColumn id="13" name="DOB" dataDxfId="6"/>
-    <tableColumn id="14" name="KTP Domisili" dataDxfId="5"/>
-    <tableColumn id="15" name="Join Date" dataDxfId="4"/>
-    <tableColumn id="16" name="Pendidikan" dataDxfId="3"/>
-    <tableColumn id="18" name="Status" dataDxfId="2"/>
+    <tableColumn id="6" name="Address" dataDxfId="10"/>
+    <tableColumn id="7" name="Address Code" dataDxfId="9"/>
+    <tableColumn id="8" name="Job" dataDxfId="8"/>
+    <tableColumn id="9" name="Salary Range" dataDxfId="7"/>
+    <tableColumn id="10" name="Phone" dataDxfId="6"/>
+    <tableColumn id="12" name="Email" dataDxfId="5"/>
+    <tableColumn id="13" name="DOB" dataDxfId="4"/>
+    <tableColumn id="14" name="KTP Domisili" dataDxfId="3"/>
+    <tableColumn id="15" name="Join Date" dataDxfId="2"/>
+    <tableColumn id="16" name="Pendidikan" dataDxfId="1"/>
+    <tableColumn id="18" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Inventory List" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -619,10 +737,10 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="17.25" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" customWidth="1"/>
@@ -637,7 +755,7 @@
     <col min="11" max="11" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="37.5" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -690,7 +808,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="17.25" customHeight="1">
       <c r="A2" s="4">
         <v>1234567</v>
       </c>
@@ -745,12 +863,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:J2">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="19" priority="2">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:I2">
-    <cfRule type="expression" dxfId="0" priority="6">
+    <cfRule type="expression" dxfId="18" priority="6">
       <formula>$J2="yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -760,6 +878,356 @@
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="7.140625" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="7">
+        <v>2</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="7">
+        <v>3</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="7">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="7">
+        <v>5</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="7">
+        <v>6</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="7">
+        <v>7</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="7">
+        <v>8</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="7">
+        <v>2</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="7">
+        <v>3</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="7">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="7">
+        <v>5</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="7">
+        <v>6</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="7">
+        <v>8</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="7">
+        <v>9</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="7">
+        <v>10</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="7">
+        <v>11</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="7">
+        <v>12</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="7">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="7">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="7">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="7">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="7">
+        <v>11</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="7">
+        <v>12</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>